<commit_message>
DOMA-2542 Localization for Excel template (payments)
</commit_message>
<xml_diff>
--- a/apps/condo/domains/acquiring/templates/PaymentsExportTemplate.xlsx
+++ b/apps/condo/domains/acquiring/templates/PaymentsExportTemplate.xlsx
@@ -5,7 +5,7 @@
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Контакты" sheetId="1" r:id="rId4"/>
+    <sheet name="{d.i18n.sheetName}" sheetId="1" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
@@ -13,25 +13,25 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
   <si>
-    <t>Дата</t>
-  </si>
-  <si>
-    <t>ЛС</t>
-  </si>
-  <si>
-    <t>Адрес</t>
-  </si>
-  <si>
-    <t>Помещение</t>
-  </si>
-  <si>
-    <t>Тип</t>
-  </si>
-  <si>
-    <t>Транзакция</t>
-  </si>
-  <si>
-    <t>Сумма</t>
+    <t>{d.i18n.date}</t>
+  </si>
+  <si>
+    <t>{d.i18n.account}</t>
+  </si>
+  <si>
+    <t>{d.i18n.address}</t>
+  </si>
+  <si>
+    <t>{d.i18n.unitName}</t>
+  </si>
+  <si>
+    <t>{d.i18n.type}</t>
+  </si>
+  <si>
+    <t>{d.i18n.transaction}</t>
+  </si>
+  <si>
+    <t>{d.i18n.amount}</t>
   </si>
   <si>
     <t>{d.objs[i].date}</t>
@@ -106,7 +106,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -119,8 +119,14 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -147,37 +153,6 @@
       <left style="thin">
         <color indexed="8"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
       <right style="thin">
         <color indexed="8"/>
       </right>
@@ -187,31 +162,6 @@
       <bottom style="thin">
         <color indexed="11"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -229,82 +179,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -314,49 +195,10 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -377,7 +219,7 @@
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
       <rgbColor rgb="ffafb3b2"/>
-      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ff949494"/>
     </indexedColors>
   </colors>
@@ -577,12 +419,12 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -866,12 +708,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1440,7 +1282,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:Z10"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1452,8 +1294,8 @@
     <col min="4" max="4" width="10.5" style="1" customWidth="1"/>
     <col min="5" max="5" width="22" style="1" customWidth="1"/>
     <col min="6" max="6" width="29.3516" style="1" customWidth="1"/>
-    <col min="7" max="26" width="14.5" style="1" customWidth="1"/>
-    <col min="27" max="16384" width="14.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="14.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1">
@@ -1478,305 +1320,52 @@
       <c r="G1" t="s" s="2">
         <v>6</v>
       </c>
-      <c r="H1" s="3"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="5"/>
     </row>
     <row r="2" ht="15" customHeight="1">
-      <c r="A2" t="s" s="6">
+      <c r="A2" t="s" s="3">
         <v>7</v>
       </c>
-      <c r="B2" t="s" s="6">
+      <c r="B2" t="s" s="3">
         <v>8</v>
       </c>
-      <c r="C2" t="s" s="6">
+      <c r="C2" t="s" s="3">
         <v>9</v>
       </c>
-      <c r="D2" t="s" s="6">
+      <c r="D2" t="s" s="3">
         <v>10</v>
       </c>
-      <c r="E2" t="s" s="6">
+      <c r="E2" t="s" s="3">
         <v>11</v>
       </c>
-      <c r="F2" t="s" s="6">
+      <c r="F2" t="s" s="3">
         <v>12</v>
       </c>
-      <c r="G2" t="s" s="6">
+      <c r="G2" t="s" s="3">
         <v>13</v>
       </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
-      <c r="W2" s="8"/>
-      <c r="X2" s="8"/>
-      <c r="Y2" s="8"/>
-      <c r="Z2" s="9"/>
     </row>
     <row r="3" ht="15" customHeight="1">
-      <c r="A3" t="s" s="10">
+      <c r="A3" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="B3" t="s" s="10">
+      <c r="B3" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="C3" t="s" s="10">
+      <c r="C3" t="s" s="4">
         <v>16</v>
       </c>
-      <c r="D3" t="s" s="10">
+      <c r="D3" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="E3" t="s" s="10">
+      <c r="E3" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="F3" t="s" s="10">
+      <c r="F3" t="s" s="4">
         <v>19</v>
       </c>
-      <c r="G3" t="s" s="10">
+      <c r="G3" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="H3" s="11"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="8"/>
-      <c r="Y3" s="8"/>
-      <c r="Z3" s="9"/>
-    </row>
-    <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="12"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="8"/>
-      <c r="U4" s="8"/>
-      <c r="V4" s="8"/>
-      <c r="W4" s="8"/>
-      <c r="X4" s="8"/>
-      <c r="Y4" s="8"/>
-      <c r="Z4" s="9"/>
-    </row>
-    <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="14"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="8"/>
-      <c r="T5" s="8"/>
-      <c r="U5" s="8"/>
-      <c r="V5" s="8"/>
-      <c r="W5" s="8"/>
-      <c r="X5" s="8"/>
-      <c r="Y5" s="8"/>
-      <c r="Z5" s="9"/>
-    </row>
-    <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="14"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="8"/>
-      <c r="R6" s="8"/>
-      <c r="S6" s="8"/>
-      <c r="T6" s="8"/>
-      <c r="U6" s="8"/>
-      <c r="V6" s="8"/>
-      <c r="W6" s="8"/>
-      <c r="X6" s="8"/>
-      <c r="Y6" s="8"/>
-      <c r="Z6" s="9"/>
-    </row>
-    <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="14"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="8"/>
-      <c r="R7" s="8"/>
-      <c r="S7" s="8"/>
-      <c r="T7" s="8"/>
-      <c r="U7" s="8"/>
-      <c r="V7" s="8"/>
-      <c r="W7" s="8"/>
-      <c r="X7" s="8"/>
-      <c r="Y7" s="8"/>
-      <c r="Z7" s="9"/>
-    </row>
-    <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="14"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="8"/>
-      <c r="R8" s="8"/>
-      <c r="S8" s="8"/>
-      <c r="T8" s="8"/>
-      <c r="U8" s="8"/>
-      <c r="V8" s="8"/>
-      <c r="W8" s="8"/>
-      <c r="X8" s="8"/>
-      <c r="Y8" s="8"/>
-      <c r="Z8" s="9"/>
-    </row>
-    <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="14"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="8"/>
-      <c r="R9" s="8"/>
-      <c r="S9" s="8"/>
-      <c r="T9" s="8"/>
-      <c r="U9" s="8"/>
-      <c r="V9" s="8"/>
-      <c r="W9" s="8"/>
-      <c r="X9" s="8"/>
-      <c r="Y9" s="8"/>
-      <c r="Z9" s="9"/>
-    </row>
-    <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="15"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="16"/>
-      <c r="N10" s="16"/>
-      <c r="O10" s="16"/>
-      <c r="P10" s="16"/>
-      <c r="Q10" s="16"/>
-      <c r="R10" s="16"/>
-      <c r="S10" s="16"/>
-      <c r="T10" s="16"/>
-      <c r="U10" s="16"/>
-      <c r="V10" s="16"/>
-      <c r="W10" s="16"/>
-      <c r="X10" s="16"/>
-      <c r="Y10" s="16"/>
-      <c r="Z10" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0" footer="0"/>

</xml_diff>

<commit_message>
Revert "DOMA-2542 Localization for Excel template (payments)"
This reverts commit 77be65456b88055adef457e101dd262559d6eacb.
</commit_message>
<xml_diff>
--- a/apps/condo/domains/acquiring/templates/PaymentsExportTemplate.xlsx
+++ b/apps/condo/domains/acquiring/templates/PaymentsExportTemplate.xlsx
@@ -5,7 +5,7 @@
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="{d.i18n.sheetName}" sheetId="1" r:id="rId4"/>
+    <sheet name="Контакты" sheetId="1" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
@@ -13,25 +13,25 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
   <si>
-    <t>{d.i18n.date}</t>
-  </si>
-  <si>
-    <t>{d.i18n.account}</t>
-  </si>
-  <si>
-    <t>{d.i18n.address}</t>
-  </si>
-  <si>
-    <t>{d.i18n.unitName}</t>
-  </si>
-  <si>
-    <t>{d.i18n.type}</t>
-  </si>
-  <si>
-    <t>{d.i18n.transaction}</t>
-  </si>
-  <si>
-    <t>{d.i18n.amount}</t>
+    <t>Дата</t>
+  </si>
+  <si>
+    <t>ЛС</t>
+  </si>
+  <si>
+    <t>Адрес</t>
+  </si>
+  <si>
+    <t>Помещение</t>
+  </si>
+  <si>
+    <t>Тип</t>
+  </si>
+  <si>
+    <t>Транзакция</t>
+  </si>
+  <si>
+    <t>Сумма</t>
   </si>
   <si>
     <t>{d.objs[i].date}</t>
@@ -106,7 +106,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -119,14 +119,8 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="4">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -153,6 +147,37 @@
       <left style="thin">
         <color indexed="8"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
       <right style="thin">
         <color indexed="8"/>
       </right>
@@ -162,6 +187,31 @@
       <bottom style="thin">
         <color indexed="11"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -179,13 +229,82 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -195,10 +314,49 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -219,7 +377,7 @@
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
       <rgbColor rgb="ffafb3b2"/>
-      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ff949494"/>
     </indexedColors>
   </colors>
@@ -419,12 +577,12 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="25400" cap="flat">
+        <a:ln w="12700" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:round/>
+          <a:miter lim="800000"/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -708,12 +866,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="25400" cap="flat">
+        <a:ln w="12700" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:round/>
+          <a:miter lim="800000"/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1282,7 +1440,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:Z10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1294,8 +1452,8 @@
     <col min="4" max="4" width="10.5" style="1" customWidth="1"/>
     <col min="5" max="5" width="22" style="1" customWidth="1"/>
     <col min="6" max="6" width="29.3516" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="14.5" style="1" customWidth="1"/>
+    <col min="7" max="26" width="14.5" style="1" customWidth="1"/>
+    <col min="27" max="16384" width="14.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1">
@@ -1320,52 +1478,305 @@
       <c r="G1" t="s" s="2">
         <v>6</v>
       </c>
+      <c r="H1" s="3"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="5"/>
     </row>
     <row r="2" ht="15" customHeight="1">
-      <c r="A2" t="s" s="3">
+      <c r="A2" t="s" s="6">
         <v>7</v>
       </c>
-      <c r="B2" t="s" s="3">
+      <c r="B2" t="s" s="6">
         <v>8</v>
       </c>
-      <c r="C2" t="s" s="3">
+      <c r="C2" t="s" s="6">
         <v>9</v>
       </c>
-      <c r="D2" t="s" s="3">
+      <c r="D2" t="s" s="6">
         <v>10</v>
       </c>
-      <c r="E2" t="s" s="3">
+      <c r="E2" t="s" s="6">
         <v>11</v>
       </c>
-      <c r="F2" t="s" s="3">
+      <c r="F2" t="s" s="6">
         <v>12</v>
       </c>
-      <c r="G2" t="s" s="3">
+      <c r="G2" t="s" s="6">
         <v>13</v>
       </c>
+      <c r="H2" s="7"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="9"/>
     </row>
     <row r="3" ht="15" customHeight="1">
-      <c r="A3" t="s" s="4">
+      <c r="A3" t="s" s="10">
         <v>14</v>
       </c>
-      <c r="B3" t="s" s="4">
+      <c r="B3" t="s" s="10">
         <v>15</v>
       </c>
-      <c r="C3" t="s" s="4">
+      <c r="C3" t="s" s="10">
         <v>16</v>
       </c>
-      <c r="D3" t="s" s="4">
+      <c r="D3" t="s" s="10">
         <v>17</v>
       </c>
-      <c r="E3" t="s" s="4">
+      <c r="E3" t="s" s="10">
         <v>18</v>
       </c>
-      <c r="F3" t="s" s="4">
+      <c r="F3" t="s" s="10">
         <v>19</v>
       </c>
-      <c r="G3" t="s" s="4">
+      <c r="G3" t="s" s="10">
         <v>20</v>
       </c>
+      <c r="H3" s="11"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="9"/>
+    </row>
+    <row r="4" ht="13.65" customHeight="1">
+      <c r="A4" s="12"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
+      <c r="Y4" s="8"/>
+      <c r="Z4" s="9"/>
+    </row>
+    <row r="5" ht="13.65" customHeight="1">
+      <c r="A5" s="14"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
+      <c r="Y5" s="8"/>
+      <c r="Z5" s="9"/>
+    </row>
+    <row r="6" ht="13.65" customHeight="1">
+      <c r="A6" s="14"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="8"/>
+      <c r="S6" s="8"/>
+      <c r="T6" s="8"/>
+      <c r="U6" s="8"/>
+      <c r="V6" s="8"/>
+      <c r="W6" s="8"/>
+      <c r="X6" s="8"/>
+      <c r="Y6" s="8"/>
+      <c r="Z6" s="9"/>
+    </row>
+    <row r="7" ht="13.65" customHeight="1">
+      <c r="A7" s="14"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="8"/>
+      <c r="S7" s="8"/>
+      <c r="T7" s="8"/>
+      <c r="U7" s="8"/>
+      <c r="V7" s="8"/>
+      <c r="W7" s="8"/>
+      <c r="X7" s="8"/>
+      <c r="Y7" s="8"/>
+      <c r="Z7" s="9"/>
+    </row>
+    <row r="8" ht="13.65" customHeight="1">
+      <c r="A8" s="14"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="8"/>
+      <c r="S8" s="8"/>
+      <c r="T8" s="8"/>
+      <c r="U8" s="8"/>
+      <c r="V8" s="8"/>
+      <c r="W8" s="8"/>
+      <c r="X8" s="8"/>
+      <c r="Y8" s="8"/>
+      <c r="Z8" s="9"/>
+    </row>
+    <row r="9" ht="13.65" customHeight="1">
+      <c r="A9" s="14"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="8"/>
+      <c r="T9" s="8"/>
+      <c r="U9" s="8"/>
+      <c r="V9" s="8"/>
+      <c r="W9" s="8"/>
+      <c r="X9" s="8"/>
+      <c r="Y9" s="8"/>
+      <c r="Z9" s="9"/>
+    </row>
+    <row r="10" ht="13.65" customHeight="1">
+      <c r="A10" s="15"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="16"/>
+      <c r="R10" s="16"/>
+      <c r="S10" s="16"/>
+      <c r="T10" s="16"/>
+      <c r="U10" s="16"/>
+      <c r="V10" s="16"/>
+      <c r="W10" s="16"/>
+      <c r="X10" s="16"/>
+      <c r="Y10" s="16"/>
+      <c r="Z10" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0" footer="0"/>

</xml_diff>

<commit_message>
DOMA-3382 add payment status to excel export
-update templates
-update ExportPaymentsService
</commit_message>
<xml_diff>
--- a/apps/condo/domains/acquiring/templates/PaymentsExportTemplate.xlsx
+++ b/apps/condo/domains/acquiring/templates/PaymentsExportTemplate.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
   <si>
     <t>{d.i18n.date}</t>
   </si>
@@ -31,6 +31,9 @@
     <t>{d.i18n.transaction}</t>
   </si>
   <si>
+    <t>{d.i18n.status}</t>
+  </si>
+  <si>
     <t>{d.i18n.amount}</t>
   </si>
   <si>
@@ -52,6 +55,9 @@
     <t>{d.objs[i].transaction}</t>
   </si>
   <si>
+    <t>{d.objs[I].status}</t>
+  </si>
+  <si>
     <t>{d.objs[i].amount}</t>
   </si>
   <si>
@@ -71,6 +77,9 @@
   </si>
   <si>
     <t>{d.objs[i+1].transaction}</t>
+  </si>
+  <si>
+    <t>{d.objs[i+1].status}</t>
   </si>
   <si>
     <t>{d.objs[i+1].amount}</t>
@@ -90,9 +99,9 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="15"/>
+      <sz val="13"/>
       <color indexed="8"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
     </font>
     <font>
       <b val="1"/>
@@ -126,7 +135,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -179,13 +188,100 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -199,6 +295,33 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -221,6 +344,7 @@
       <rgbColor rgb="ffafb3b2"/>
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ff949494"/>
+      <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1282,7 +1406,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1294,8 +1418,8 @@
     <col min="4" max="4" width="10.5" style="1" customWidth="1"/>
     <col min="5" max="5" width="22" style="1" customWidth="1"/>
     <col min="6" max="6" width="29.3516" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="14.5" style="1" customWidth="1"/>
+    <col min="7" max="8" width="14.5" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="14.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1">
@@ -1320,52 +1444,131 @@
       <c r="G1" t="s" s="2">
         <v>6</v>
       </c>
+      <c r="H1" t="s" s="2">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" ht="15" customHeight="1">
       <c r="A2" t="s" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s" s="3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s" s="3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s" s="3">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s" s="3">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="H2" t="s" s="3">
+        <v>15</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1">
       <c r="A3" t="s" s="4">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s" s="4">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s" s="4">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s" s="4">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s" s="4">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F3" t="s" s="4">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G3" t="s" s="4">
-        <v>20</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="H3" t="s" s="4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" ht="13.65" customHeight="1">
+      <c r="A4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="7"/>
+    </row>
+    <row r="5" ht="13.65" customHeight="1">
+      <c r="A5" s="8"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="10"/>
+    </row>
+    <row r="6" ht="13.65" customHeight="1">
+      <c r="A6" s="8"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="10"/>
+    </row>
+    <row r="7" ht="13.65" customHeight="1">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="10"/>
+    </row>
+    <row r="8" ht="13.65" customHeight="1">
+      <c r="A8" s="8"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="10"/>
+    </row>
+    <row r="9" ht="13.65" customHeight="1">
+      <c r="A9" s="8"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="10"/>
+    </row>
+    <row r="10" ht="13.65" customHeight="1">
+      <c r="A10" s="11"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0" footer="0"/>

</xml_diff>

<commit_message>
feat(condo): DOMA-4173 add new columns in excel export
</commit_message>
<xml_diff>
--- a/apps/condo/domains/acquiring/templates/PaymentsExportTemplate.xlsx
+++ b/apps/condo/domains/acquiring/templates/PaymentsExportTemplate.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
   <si>
     <t>{d.i18n.date}</t>
   </si>
@@ -31,6 +31,9 @@
     <t>{d.i18n.transaction}</t>
   </si>
   <si>
+    <t>{d.i18n.order}</t>
+  </si>
+  <si>
     <t>{d.i18n.status}</t>
   </si>
   <si>
@@ -55,6 +58,9 @@
     <t>{d.objs[i].transaction}</t>
   </si>
   <si>
+    <t>{d.objs[I].order}</t>
+  </si>
+  <si>
     <t>{d.objs[I].status}</t>
   </si>
   <si>
@@ -77,6 +83,9 @@
   </si>
   <si>
     <t>{d.objs[i+1].transaction}</t>
+  </si>
+  <si>
+    <t>{d.objs[I+1].order}</t>
   </si>
   <si>
     <t>{d.objs[i+1].status}</t>
@@ -1406,7 +1415,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1418,8 +1427,9 @@
     <col min="4" max="4" width="10.5" style="1" customWidth="1"/>
     <col min="5" max="5" width="22" style="1" customWidth="1"/>
     <col min="6" max="6" width="29.3516" style="1" customWidth="1"/>
-    <col min="7" max="8" width="14.5" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="14.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="25.9375" style="1" customWidth="1"/>
+    <col min="8" max="9" width="14.5" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="14.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1">
@@ -1447,57 +1457,66 @@
       <c r="H1" t="s" s="2">
         <v>7</v>
       </c>
+      <c r="I1" t="s" s="2">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" ht="15" customHeight="1">
       <c r="A2" t="s" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s" s="3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s" s="3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s" s="3">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" t="s" s="3">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G2" t="s" s="3">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H2" t="s" s="3">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="I2" t="s" s="3">
+        <v>17</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1">
       <c r="A3" t="s" s="4">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s" s="4">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s" s="4">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s" s="4">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s" s="4">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F3" t="s" s="4">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G3" t="s" s="4">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H3" t="s" s="4">
-        <v>23</v>
+        <v>25</v>
+      </c>
+      <c r="I3" t="s" s="4">
+        <v>26</v>
       </c>
     </row>
     <row r="4" ht="13.65" customHeight="1">
@@ -1508,7 +1527,8 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
-      <c r="H4" s="7"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="7"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
       <c r="A5" s="8"/>
@@ -1518,7 +1538,8 @@
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
-      <c r="H5" s="10"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="10"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
       <c r="A6" s="8"/>
@@ -1528,7 +1549,8 @@
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
-      <c r="H6" s="10"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="10"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
       <c r="A7" s="8"/>
@@ -1538,7 +1560,8 @@
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
-      <c r="H7" s="10"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="10"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
       <c r="A8" s="8"/>
@@ -1548,7 +1571,8 @@
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
-      <c r="H8" s="10"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="10"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
       <c r="A9" s="8"/>
@@ -1558,7 +1582,8 @@
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
-      <c r="H9" s="10"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="10"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
@@ -1568,7 +1593,8 @@
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
       <c r="G10" s="12"/>
-      <c r="H10" s="13"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0" footer="0"/>

</xml_diff>

<commit_message>
feat(condo): DOMA-8440 add invoice number to payments export
</commit_message>
<xml_diff>
--- a/apps/condo/domains/acquiring/templates/PaymentsExportTemplate.xlsx
+++ b/apps/condo/domains/acquiring/templates/PaymentsExportTemplate.xlsx
@@ -1,21 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{50DCD77A-3C14-4616-BCF4-5BED184F669D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="{d.i18n.sheetName}" sheetId="1" r:id="rId4"/>
+    <sheet name="{d.i18n.sheetName}" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="191028" refMode="R1C1" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>{d.i18n.date}</t>
   </si>
   <si>
+    <t>{d.i18n.invoiceNumber}</t>
+  </si>
+  <si>
     <t>{d.i18n.account}</t>
   </si>
   <si>
@@ -43,6 +66,9 @@
     <t>{d.objs[i].date}</t>
   </si>
   <si>
+    <t>{d.objs[i].invoiceNumber}</t>
+  </si>
+  <si>
     <t>{d.objs[i].account}</t>
   </si>
   <si>
@@ -64,12 +90,15 @@
     <t>{d.objs[I].status}</t>
   </si>
   <si>
-    <t>{d.objs[i].amount}</t>
+    <t>{d.objs[I].amount}</t>
   </si>
   <si>
     <t>{d.objs[i+1].date}</t>
   </si>
   <si>
+    <t>{d.objs[i+1].invoiceNumber}</t>
+  </si>
+  <si>
     <t>{d.objs[i+1].account}</t>
   </si>
   <si>
@@ -91,29 +120,21 @@
     <t>{d.objs[i+1].status}</t>
   </si>
   <si>
-    <t>{d.objs[i+1].amount}</t>
+    <t>{d.objs[I+1].amount}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="13"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b val="1"/>
+      <b/>
       <sz val="8"/>
       <color indexed="8"/>
       <name val="Arial"/>
@@ -144,7 +165,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -219,148 +240,126 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color indexed="12"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="12"/>
-      </left>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="12"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="11"/>
       </left>
       <right/>
-      <top/>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
       <bottom style="thin">
-        <color indexed="12"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="12"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="12"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="8"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+  <cellXfs count="10">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffafb3b2"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ff949494"/>
-      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFAFB3B2"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FF949494"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -562,7 +561,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -581,7 +580,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -611,7 +610,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -637,7 +636,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -663,7 +662,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -689,7 +688,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -715,7 +714,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -741,7 +740,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -767,7 +766,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -793,7 +792,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -819,7 +818,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -832,9 +831,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -851,7 +856,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -870,7 +875,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -896,7 +901,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -922,7 +927,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -948,7 +953,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -974,7 +979,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1000,7 +1005,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1026,7 +1031,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1052,7 +1057,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1078,7 +1083,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1104,7 +1109,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1117,9 +1122,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1133,7 +1144,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1152,7 +1163,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1182,7 +1193,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1208,7 +1219,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1234,7 +1245,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1260,7 +1271,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1286,7 +1297,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1312,7 +1323,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1338,7 +1349,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1364,7 +1375,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1390,7 +1401,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1403,123 +1414,141 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="37.8516" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.6719" style="1" customWidth="1"/>
-    <col min="3" max="3" width="35.8516" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="37.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="35.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="22" style="1" customWidth="1"/>
-    <col min="6" max="6" width="29.3516" style="1" customWidth="1"/>
-    <col min="7" max="7" width="25.9375" style="1" customWidth="1"/>
-    <col min="8" max="9" width="14.5" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="14.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="29.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="26" style="1" customWidth="1"/>
+    <col min="8" max="10" width="14.42578125" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="14.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:10" ht="15" customHeight="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="2">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="2">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="2">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s" s="2">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" ht="15" customHeight="1">
-      <c r="A2" t="s" s="3">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s" s="3">
+    <row r="2" spans="1:10" ht="15" customHeight="1">
+      <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s" s="3">
+      <c r="B2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s" s="3">
+      <c r="C2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s" s="3">
+      <c r="D2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F2" t="s" s="3">
+      <c r="E2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G2" t="s" s="3">
+      <c r="F2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H2" t="s" s="3">
+      <c r="G2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I2" t="s" s="3">
+      <c r="H2" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="I2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="3" ht="15" customHeight="1">
-      <c r="A3" t="s" s="4">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s" s="4">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s" s="4">
+    <row r="3" spans="1:10" ht="15" customHeight="1">
+      <c r="A3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D3" t="s" s="4">
+      <c r="B3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E3" t="s" s="4">
+      <c r="C3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F3" t="s" s="4">
+      <c r="D3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G3" t="s" s="4">
+      <c r="E3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H3" t="s" s="4">
+      <c r="F3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I3" t="s" s="4">
+      <c r="G3" s="4" t="s">
         <v>26</v>
       </c>
+      <c r="H3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="4" ht="13.65" customHeight="1">
+    <row r="4" spans="1:10" ht="13.7" customHeight="1">
       <c r="A4" s="5"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -1529,76 +1558,143 @@
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
       <c r="I4" s="7"/>
+      <c r="J4" s="8"/>
     </row>
-    <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="8"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="10"/>
+    <row r="5" spans="1:10" ht="13.7" customHeight="1">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
     </row>
-    <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="8"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="10"/>
+    <row r="6" spans="1:10" ht="13.7" customHeight="1">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
     </row>
-    <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="10"/>
+    <row r="7" spans="1:10" ht="13.7" customHeight="1">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
     </row>
-    <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="10"/>
+    <row r="8" spans="1:10" ht="13.7" customHeight="1">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
     </row>
-    <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="8"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="10"/>
+    <row r="9" spans="1:10" ht="13.7" customHeight="1">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
     </row>
-    <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="11"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="13"/>
+    <row r="10" spans="1:10" ht="13.7" customHeight="1">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+    </row>
+    <row r="11" spans="1:10" ht="15" customHeight="1">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+    </row>
+    <row r="12" spans="1:10" ht="15" customHeight="1">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+    </row>
+    <row r="13" spans="1:10" ht="15" customHeight="1">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+    </row>
+    <row r="14" spans="1:10" ht="15" customHeight="1">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+    </row>
+    <row r="15" spans="1:10" ht="15" customHeight="1">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
     </row>
   </sheetData>
-  <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0" footer="0"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageMargins left="0.74791700000000005" right="0.74791700000000005" top="0.98402800000000001" bottom="0.98402800000000001" header="0" footer="0"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Arial,Regular"&amp;10&amp;K000000000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>